<commit_message>
Updated contact form and layout
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj\OneDrive\Desktop\AptiPi Technologies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E2E113-10D7-4F4D-9847-AA269B234299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA68457-BA64-4C8B-B66C-0DCCF68729E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -40,7 +40,13 @@
     <t>manojmd780@gmail.com</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Manoj M D</t>
+  </si>
+  <si>
+    <t>+919972028266</t>
+  </si>
+  <si>
+    <t>yuhfdga</t>
   </si>
 </sst>
 </file>
@@ -96,13 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,19 +409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -436,28 +438,39 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>9972028267</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>2334567888</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>